<commit_message>
listados completos del 19 de agosto
</commit_message>
<xml_diff>
--- a/Agosto/16 agosto/matehuala/PLANTILLA LISTA DE ASPIRANTES_MATEHUALA(ESPECIAL).xlsx
+++ b/Agosto/16 agosto/matehuala/PLANTILLA LISTA DE ASPIRANTES_MATEHUALA(ESPECIAL).xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Proyecto01TICs\Documents\Evaluatec2024\Agosto\16 agosto\matehuala\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MaxoC\OneDrive\Documents\EVALUATEC2024\Agosto\16 agosto\matehuala\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CC41EE0-0D27-4ABD-9FC8-9BB2DC23FDE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{495AE668-3740-4E1C-9C7A-3EAB5D5ABE09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D610CFFB-2790-104B-A52B-2B33694C28D9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D610CFFB-2790-104B-A52B-2B33694C28D9}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="78">
   <si>
     <t xml:space="preserve">b </t>
   </si>
@@ -246,21 +246,6 @@
     <t>soalmen14@gmail.com</t>
   </si>
   <si>
-    <t>COPU-2010-206</t>
-  </si>
-  <si>
-    <t>COPU-2010-207</t>
-  </si>
-  <si>
-    <t>IIND-2010-228</t>
-  </si>
-  <si>
-    <t>IIND-2010-229</t>
-  </si>
-  <si>
-    <t>IIND-2010-230</t>
-  </si>
-  <si>
     <t>ALEJO LOERA ANDREA CAMILA</t>
   </si>
   <si>
@@ -473,7 +458,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -539,7 +524,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="2" applyBorder="1"/>
     <xf numFmtId="18" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -551,6 +535,10 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="2" applyBorder="1"/>
+    <xf numFmtId="18" fontId="8" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -608,6 +596,9 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{5925BC7A-0E73-734D-A0C9-B8A68F88FF64}" name="Tabla2" displayName="Tabla2" ref="A4:M443" totalsRowShown="0">
   <autoFilter ref="A4:M443" xr:uid="{5925BC7A-0E73-734D-A0C9-B8A68F88FF64}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:M443">
+    <sortCondition ref="E4:E443"/>
+  </sortState>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{F5111305-CA2B-DF41-BA05-5C9A177B7523}" name="FICHA"/>
     <tableColumn id="2" xr3:uid="{D956ADB6-2882-CB4B-9C6B-032AC358A5C1}" name="NOMBRE ASPIRANTE"/>
@@ -927,7 +918,7 @@
   <dimension ref="A1:O443"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:A20"/>
+      <selection activeCell="E17" sqref="E17:E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -951,25 +942,25 @@
       <c r="D1" t="s">
         <v>0</v>
       </c>
-      <c r="L1" s="35" t="s">
+      <c r="L1" s="34" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C2" s="33" t="s">
+      <c r="C2" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
-      <c r="I2" s="33"/>
-      <c r="J2" s="33"/>
-      <c r="L2" s="35"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
+      <c r="L2" s="34"/>
     </row>
     <row r="3" spans="1:15" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="L3" s="35"/>
+      <c r="L3" s="34"/>
     </row>
     <row r="4" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -1061,7 +1052,7 @@
         <v>26</v>
       </c>
       <c r="E6" s="21" t="s">
-        <v>73</v>
+        <v>18</v>
       </c>
       <c r="F6" t="s">
         <v>29</v>
@@ -1081,8 +1072,8 @@
         <v>22</v>
       </c>
       <c r="M6" s="14"/>
-      <c r="N6" s="34"/>
-      <c r="O6" s="34"/>
+      <c r="N6" s="33"/>
+      <c r="O6" s="33"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="27">
@@ -1098,7 +1089,7 @@
         <v>34</v>
       </c>
       <c r="E7" s="21" t="s">
-        <v>74</v>
+        <v>18</v>
       </c>
       <c r="F7" s="24" t="s">
         <v>29</v>
@@ -1121,24 +1112,24 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="27">
-        <v>24660449</v>
+        <v>24660485</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>35</v>
+        <v>74</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>37</v>
+        <v>76</v>
+      </c>
+      <c r="D8" s="35" t="s">
+        <v>77</v>
       </c>
       <c r="E8" s="21" t="s">
-        <v>19</v>
+        <v>75</v>
       </c>
       <c r="F8" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="G8" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="G8" s="30" t="s">
         <v>15</v>
       </c>
       <c r="H8" s="13"/>
@@ -1146,32 +1137,32 @@
       <c r="J8" s="13">
         <v>45520</v>
       </c>
-      <c r="K8" s="26" t="s">
+      <c r="K8" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="L8" s="26" t="s">
+      <c r="L8" s="31" t="s">
         <v>22</v>
       </c>
       <c r="M8" s="25"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="27">
-        <v>24660435</v>
+        <v>24660449</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E9" s="21" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="F9" s="24" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="G9" s="18" t="s">
         <v>15</v>
@@ -1191,22 +1182,22 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="27">
-        <v>24660446</v>
+        <v>24660484</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>42</v>
+        <v>70</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>43</v>
+        <v>71</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>44</v>
+        <v>72</v>
       </c>
       <c r="E10" s="21" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="F10" s="24" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="G10" s="18" t="s">
         <v>15</v>
@@ -1226,21 +1217,21 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="28">
-        <v>24660448</v>
+        <v>24660435</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="E11" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="F11" s="16" t="s">
+      <c r="F11" s="17" t="s">
         <v>39</v>
       </c>
       <c r="G11" s="18" t="s">
@@ -1257,20 +1248,20 @@
       <c r="L11" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="M11" s="14"/>
+      <c r="M11" s="15"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="27">
-        <v>24660478</v>
+        <v>24660446</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E12" s="21" t="s">
         <v>14</v>
@@ -1292,20 +1283,20 @@
       <c r="L12" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="M12" s="14"/>
+      <c r="M12" s="15"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="28">
-        <v>24660479</v>
+        <v>24660448</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>78</v>
+        <v>45</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="D13" s="16" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="E13" s="21" t="s">
         <v>14</v>
@@ -1331,22 +1322,22 @@
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="27">
-        <v>24660477</v>
+        <v>24660478</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="E14" s="21" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F14" s="24" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="G14" s="18" t="s">
         <v>15</v>
@@ -1362,26 +1353,26 @@
       <c r="L14" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="M14" s="25"/>
+      <c r="M14" s="36"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="29">
-        <v>24660480</v>
+        <v>24660479</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>57</v>
+        <v>73</v>
       </c>
       <c r="C15" s="19" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="D15" s="19" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="E15" s="21" t="s">
-        <v>75</v>
+        <v>14</v>
       </c>
       <c r="F15" s="19" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="G15" s="18" t="s">
         <v>15</v>
@@ -1401,19 +1392,19 @@
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="28">
-        <v>24660481</v>
+        <v>24660477</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="C16" s="16" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D16" s="16" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="E16" s="21" t="s">
-        <v>76</v>
+        <v>17</v>
       </c>
       <c r="F16" s="17" t="s">
         <v>54</v>
@@ -1436,21 +1427,21 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="28">
-        <v>24660483</v>
+        <v>24660480</v>
       </c>
       <c r="B17" s="16" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="C17" s="16" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="D17" s="16" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="E17" s="21" t="s">
-        <v>77</v>
-      </c>
-      <c r="F17" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="F17" s="16" t="s">
         <v>54</v>
       </c>
       <c r="G17" s="18" t="s">
@@ -1467,26 +1458,26 @@
       <c r="L17" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="M17" s="15"/>
+      <c r="M17" s="14"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="28">
-        <v>24660482</v>
+        <v>24660481</v>
       </c>
       <c r="B18" s="16" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C18" s="16" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="D18" s="16" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="E18" s="21" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="F18" s="17" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="G18" s="18" t="s">
         <v>15</v>
@@ -1506,22 +1497,22 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="28">
-        <v>24660484</v>
+        <v>24660483</v>
       </c>
       <c r="B19" s="16" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="C19" s="16" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="D19" s="16" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="E19" s="21" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F19" s="17" t="s">
-        <v>27</v>
+        <v>54</v>
       </c>
       <c r="G19" s="18" t="s">
         <v>15</v>
@@ -1541,24 +1532,24 @@
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="28">
-        <v>24660485</v>
+        <v>24660482</v>
       </c>
       <c r="B20" s="16" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
       <c r="C20" s="16" t="s">
-        <v>81</v>
-      </c>
-      <c r="D20" s="31" t="s">
-        <v>82</v>
+        <v>68</v>
+      </c>
+      <c r="D20" s="16" t="s">
+        <v>69</v>
       </c>
       <c r="E20" s="21" t="s">
-        <v>80</v>
+        <v>20</v>
       </c>
       <c r="F20" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="G20" s="30" t="s">
+        <v>67</v>
+      </c>
+      <c r="G20" s="18" t="s">
         <v>15</v>
       </c>
       <c r="H20" s="13"/>
@@ -1566,10 +1557,10 @@
       <c r="J20" s="13">
         <v>45520</v>
       </c>
-      <c r="K20" s="32" t="s">
+      <c r="K20" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="L20" s="32" t="s">
+      <c r="L20" s="26" t="s">
         <v>22</v>
       </c>
       <c r="M20" s="15"/>
@@ -7770,7 +7761,7 @@
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="D20" r:id="rId1" xr:uid="{F909AFDB-650F-4BAA-ACBC-54A8DA76F0EB}"/>
+    <hyperlink ref="D8" r:id="rId1" xr:uid="{F909AFDB-650F-4BAA-ACBC-54A8DA76F0EB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>